<commit_message>
style: 修改 PO 模版
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/po.xlsx
+++ b/src/main/resources/templates/excel/po.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rick/Space/Workspace/sharp-admin/src/main/resources/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A3784-330E-FB47-9C4E-FFA4D3E3B51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105943DB-3708-E344-8F45-BD7CA3929CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="760" windowWidth="32940" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>序号</t>
-  </si>
-  <si>
-    <t>资材编号</t>
   </si>
   <si>
     <t>品 名</t>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>6）保固期：24个月。</t>
+  </si>
+  <si>
+    <t>物料编号</t>
   </si>
 </sst>
 </file>
@@ -716,6 +716,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -733,45 +772,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1267,62 +1267,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
       <c r="G3" s="37"/>
       <c r="H3" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="36"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A4" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="A4" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="21.75" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -1381,12 +1381,12 @@
       <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="7"/>
       <c r="H9" s="1" t="s">
         <v>13</v>
@@ -1399,42 +1399,42 @@
       </c>
       <c r="E10" s="9"/>
       <c r="G10" s="39"/>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
     </row>
     <row r="11" spans="1:10" ht="24" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="I11" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="61" customHeight="1">
@@ -1450,50 +1450,50 @@
       <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="21" customHeight="1">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" customHeight="1">
+      <c r="A14" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1">
-      <c r="A14" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
     </row>
     <row r="15" spans="1:10" ht="21" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="73"/>
+        <v>38</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:10" ht="20.25" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="17" spans="1:30" ht="20.25" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="18" spans="1:30" ht="20.25" customHeight="1">
       <c r="A18" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="19" spans="1:30" ht="20.25" customHeight="1">
       <c r="A19" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="20" spans="1:30" ht="20.25" customHeight="1">
       <c r="A20" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="21" spans="1:30" ht="20.25" customHeight="1">
       <c r="A21" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1576,22 +1576,22 @@
       <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:30" ht="20.25" customHeight="1">
-      <c r="A22" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
+      <c r="A22" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="65"/>
     </row>
     <row r="23" spans="1:30" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="24" spans="1:30" s="4" customFormat="1" ht="20.25" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1">
       <c r="A25" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="26" spans="1:30" ht="20.25" customHeight="1">
       <c r="A26" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="27" spans="1:30" ht="20.25" customHeight="1">
       <c r="A27" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="4"/>
@@ -1687,18 +1687,18 @@
       <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:30" s="4" customFormat="1" ht="29" customHeight="1">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="52" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="52" t="s">
-        <v>37</v>
       </c>
       <c r="E28" s="53"/>
       <c r="F28" s="54"/>
       <c r="G28" s="52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="52"/>
       <c r="I28" s="50"/>
@@ -1759,6 +1759,11 @@
     <row r="30" spans="1:30" ht="42" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="H10:J10"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:J13"/>
@@ -1766,11 +1771,6 @@
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="A22:J22"/>
     <mergeCell ref="B15:J15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="H10:J10"/>
   </mergeCells>
   <pageMargins left="0.39305555555555555" right="0.18" top="0.31" bottom="0" header="0.28000000000000003" footer="0.35"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="360"/>

</xml_diff>